<commit_message>
Wrote the future work section
</commit_message>
<xml_diff>
--- a/Data Structures/hash_table/hash_table_data.xlsx
+++ b/Data Structures/hash_table/hash_table_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="202">
   <si>
     <t>cycles</t>
   </si>
@@ -772,11 +772,11 @@
     <xf numFmtId="11" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1100,11 +1100,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105419904"/>
-        <c:axId val="105421824"/>
+        <c:axId val="99128448"/>
+        <c:axId val="99130368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105419904"/>
+        <c:axId val="99128448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,7 +1133,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105421824"/>
+        <c:crossAx val="99130368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1141,7 +1141,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105421824"/>
+        <c:axId val="99130368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,7 +1171,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105419904"/>
+        <c:crossAx val="99128448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1501,11 +1501,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112795648"/>
-        <c:axId val="112797568"/>
+        <c:axId val="107697664"/>
+        <c:axId val="107699584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112795648"/>
+        <c:axId val="107697664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1534,7 +1534,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112797568"/>
+        <c:crossAx val="107699584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1542,7 +1542,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112797568"/>
+        <c:axId val="107699584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,7 +1572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112795648"/>
+        <c:crossAx val="107697664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1820,11 +1820,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112806912"/>
-        <c:axId val="112829568"/>
+        <c:axId val="107721472"/>
+        <c:axId val="107723392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112806912"/>
+        <c:axId val="107721472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1853,7 +1853,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112829568"/>
+        <c:crossAx val="107723392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1861,7 +1861,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112829568"/>
+        <c:axId val="107723392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1891,7 +1891,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112806912"/>
+        <c:crossAx val="107721472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2142,11 +2142,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112933120"/>
-        <c:axId val="112939392"/>
+        <c:axId val="107835776"/>
+        <c:axId val="107837696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112933120"/>
+        <c:axId val="107835776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2175,7 +2175,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112939392"/>
+        <c:crossAx val="107837696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2183,7 +2183,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112939392"/>
+        <c:axId val="107837696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,7 +2213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112933120"/>
+        <c:crossAx val="107835776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2546,11 +2546,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112969984"/>
-        <c:axId val="112980352"/>
+        <c:axId val="107938560"/>
+        <c:axId val="107940480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112969984"/>
+        <c:axId val="107938560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2579,7 +2579,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112980352"/>
+        <c:crossAx val="107940480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2587,7 +2587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112980352"/>
+        <c:axId val="107940480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2617,7 +2617,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112969984"/>
+        <c:crossAx val="107938560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2950,11 +2950,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113088768"/>
-        <c:axId val="113107328"/>
+        <c:axId val="107996288"/>
+        <c:axId val="107998208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113088768"/>
+        <c:axId val="107996288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2983,7 +2983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113107328"/>
+        <c:crossAx val="107998208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2991,7 +2991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113107328"/>
+        <c:axId val="107998208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3021,7 +3021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113088768"/>
+        <c:crossAx val="107996288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -3354,11 +3354,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113129728"/>
-        <c:axId val="113144192"/>
+        <c:axId val="108037632"/>
+        <c:axId val="108039552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113129728"/>
+        <c:axId val="108037632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3387,7 +3387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113144192"/>
+        <c:crossAx val="108039552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3395,7 +3395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113144192"/>
+        <c:axId val="108039552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3425,7 +3425,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113129728"/>
+        <c:crossAx val="108037632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3755,11 +3755,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113162880"/>
-        <c:axId val="113173248"/>
+        <c:axId val="108070784"/>
+        <c:axId val="108077056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113162880"/>
+        <c:axId val="108070784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3788,7 +3788,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113173248"/>
+        <c:crossAx val="108077056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3796,7 +3796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113173248"/>
+        <c:axId val="108077056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3826,7 +3826,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113162880"/>
+        <c:crossAx val="108070784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -4159,11 +4159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113212032"/>
-        <c:axId val="113222400"/>
+        <c:axId val="108128512"/>
+        <c:axId val="107348352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113212032"/>
+        <c:axId val="108128512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4192,7 +4192,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113222400"/>
+        <c:crossAx val="107348352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4200,7 +4200,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113222400"/>
+        <c:axId val="107348352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4230,7 +4230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113212032"/>
+        <c:crossAx val="108128512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4560,11 +4560,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106240640"/>
-        <c:axId val="106259200"/>
+        <c:axId val="107383040"/>
+        <c:axId val="107405696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106240640"/>
+        <c:axId val="107383040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4593,7 +4593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106259200"/>
+        <c:crossAx val="107405696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4601,7 +4601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106259200"/>
+        <c:axId val="107405696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4631,7 +4631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106240640"/>
+        <c:crossAx val="107383040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -4964,11 +4964,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106297984"/>
-        <c:axId val="106169088"/>
+        <c:axId val="107485824"/>
+        <c:axId val="107492096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106297984"/>
+        <c:axId val="107485824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4997,7 +4997,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106169088"/>
+        <c:crossAx val="107492096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5005,7 +5005,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106169088"/>
+        <c:axId val="107492096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5035,7 +5035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106297984"/>
+        <c:crossAx val="107485824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5369,11 +5369,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105673856"/>
-        <c:axId val="105675776"/>
+        <c:axId val="99320960"/>
+        <c:axId val="99322880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105673856"/>
+        <c:axId val="99320960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5402,7 +5402,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105675776"/>
+        <c:crossAx val="99322880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5410,7 +5410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105675776"/>
+        <c:axId val="99322880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5440,7 +5440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105673856"/>
+        <c:crossAx val="99320960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5770,11 +5770,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106187776"/>
-        <c:axId val="106198144"/>
+        <c:axId val="107523072"/>
+        <c:axId val="107529344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106187776"/>
+        <c:axId val="107523072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5803,7 +5803,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106198144"/>
+        <c:crossAx val="107529344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5811,7 +5811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106198144"/>
+        <c:axId val="107529344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5841,7 +5841,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106187776"/>
+        <c:crossAx val="107523072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -6174,11 +6174,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113519616"/>
-        <c:axId val="113521792"/>
+        <c:axId val="113413504"/>
+        <c:axId val="113415680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113519616"/>
+        <c:axId val="113413504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6207,7 +6207,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113521792"/>
+        <c:crossAx val="113415680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6215,7 +6215,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113521792"/>
+        <c:axId val="113415680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6245,7 +6245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113519616"/>
+        <c:crossAx val="113413504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -6496,11 +6496,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="43387520"/>
-        <c:axId val="43404672"/>
+        <c:axId val="113716224"/>
+        <c:axId val="113726592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43387520"/>
+        <c:axId val="113716224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6529,7 +6529,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43404672"/>
+        <c:crossAx val="113726592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6537,7 +6537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43404672"/>
+        <c:axId val="113726592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6567,7 +6567,411 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43387520"/>
+        <c:crossAx val="113716224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lock per Bucket;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Stoker</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>; Test-and-test-and-set</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Lock Variations; Table Size 128</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$EO$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Bucket TTAS No Pause</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$EP$22:$EW$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$EP$23:$EW$23</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9147868</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9150682</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4872624</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1311896</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>760286</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>694155</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>688232</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>199899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$EO$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Bucket TTAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$EP$22:$EW$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$EP$24:$EW$24</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9183586</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7028970</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4612602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5080256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4756162</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6102068</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4600744</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4185836</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$EO$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Bucket TTAS_RELAX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$EP$22:$EW$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$EP$25:$EW$25</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9149197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6826197</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4542780</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1875650</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>755034</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>739376</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>741477</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>218215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="45266048"/>
+        <c:axId val="45267968"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="45266048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="45267968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="45267968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Millions of Iterations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="45266048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -7114,11 +7518,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106044800"/>
-        <c:axId val="106050688"/>
+        <c:axId val="107093376"/>
+        <c:axId val="107099264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106044800"/>
+        <c:axId val="107093376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7128,7 +7532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106050688"/>
+        <c:crossAx val="107099264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7136,7 +7540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106050688"/>
+        <c:axId val="107099264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7147,7 +7551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106044800"/>
+        <c:crossAx val="107093376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7723,11 +8127,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106083072"/>
-        <c:axId val="106084992"/>
+        <c:axId val="107133184"/>
+        <c:axId val="107135360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106083072"/>
+        <c:axId val="107133184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7756,7 +8160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106084992"/>
+        <c:crossAx val="107135360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7764,7 +8168,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106084992"/>
+        <c:axId val="107135360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7794,7 +8198,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106083072"/>
+        <c:crossAx val="107133184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8042,11 +8446,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105936768"/>
-        <c:axId val="105938944"/>
+        <c:axId val="106981632"/>
+        <c:axId val="106983808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105936768"/>
+        <c:axId val="106981632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8075,7 +8479,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105938944"/>
+        <c:crossAx val="106983808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8083,7 +8487,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105938944"/>
+        <c:axId val="106983808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8113,7 +8517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105936768"/>
+        <c:crossAx val="106981632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8443,11 +8847,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105965824"/>
-        <c:axId val="105968000"/>
+        <c:axId val="107014400"/>
+        <c:axId val="107016576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105965824"/>
+        <c:axId val="107014400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8476,7 +8880,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105968000"/>
+        <c:crossAx val="107016576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8484,7 +8888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105968000"/>
+        <c:axId val="107016576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8514,7 +8918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105965824"/>
+        <c:crossAx val="107014400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -8847,11 +9251,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106031360"/>
-        <c:axId val="112656768"/>
+        <c:axId val="107084416"/>
+        <c:axId val="107614976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106031360"/>
+        <c:axId val="107084416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8880,7 +9284,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112656768"/>
+        <c:crossAx val="107614976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8888,7 +9292,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112656768"/>
+        <c:axId val="107614976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8918,7 +9322,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106031360"/>
+        <c:crossAx val="107084416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -9579,11 +9983,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112702976"/>
-        <c:axId val="112704896"/>
+        <c:axId val="107663744"/>
+        <c:axId val="107665664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112702976"/>
+        <c:axId val="107663744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9612,7 +10016,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112704896"/>
+        <c:crossAx val="107665664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9620,7 +10024,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112704896"/>
+        <c:axId val="107665664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9650,7 +10054,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112702976"/>
+        <c:crossAx val="107663744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -10065,11 +10469,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112867200"/>
-        <c:axId val="112877568"/>
+        <c:axId val="107758720"/>
+        <c:axId val="107760640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112867200"/>
+        <c:axId val="107758720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10098,7 +10502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112877568"/>
+        <c:crossAx val="107760640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10106,7 +10510,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112877568"/>
+        <c:axId val="107760640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10136,7 +10540,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112867200"/>
+        <c:crossAx val="107758720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -10861,6 +11265,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>144</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>160</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="25" name="Chart 24"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -11151,10 +11587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:EJ468"/>
+  <dimension ref="A3:EZ468"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CB121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DY44" sqref="DY44:ED47"/>
+    <sheetView tabSelected="1" topLeftCell="EE13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="EO41" sqref="EO41:ET44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11196,20 +11632,23 @@
     <col min="129" max="129" width="26" customWidth="1"/>
     <col min="133" max="133" width="15.140625" customWidth="1"/>
     <col min="137" max="137" width="16.5703125" customWidth="1"/>
+    <col min="145" max="145" width="32" customWidth="1"/>
+    <col min="149" max="149" width="17.85546875" customWidth="1"/>
+    <col min="153" max="153" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B4">
@@ -11236,17 +11675,17 @@
       <c r="I4">
         <v>128</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -12165,7 +12604,7 @@
         <v>5841043</v>
       </c>
     </row>
-    <row r="17" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -12266,7 +12705,7 @@
         <v>5669610</v>
       </c>
     </row>
-    <row r="18" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -12307,7 +12746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -12335,17 +12774,17 @@
       <c r="I19" s="6">
         <v>6760276</v>
       </c>
-      <c r="K19" s="16" t="s">
+      <c r="K19" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
       <c r="W19" s="6">
         <v>197952563</v>
       </c>
@@ -12359,7 +12798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -12456,7 +12895,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -12725,7 +13164,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -13010,8 +13449,32 @@
       <c r="EG22" s="6">
         <v>4691086</v>
       </c>
-    </row>
-    <row r="23" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP22">
+        <v>1</v>
+      </c>
+      <c r="EQ22">
+        <v>2</v>
+      </c>
+      <c r="ER22">
+        <v>4</v>
+      </c>
+      <c r="ES22">
+        <v>8</v>
+      </c>
+      <c r="ET22">
+        <v>16</v>
+      </c>
+      <c r="EU22">
+        <v>32</v>
+      </c>
+      <c r="EV22">
+        <v>64</v>
+      </c>
+      <c r="EW22">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -13288,8 +13751,35 @@
       <c r="EG23" s="6">
         <v>33824</v>
       </c>
-    </row>
-    <row r="24" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EO23" t="s">
+        <v>65</v>
+      </c>
+      <c r="EP23" s="6">
+        <v>9147868</v>
+      </c>
+      <c r="EQ23" s="6">
+        <v>9150682</v>
+      </c>
+      <c r="ER23" s="6">
+        <v>4872624</v>
+      </c>
+      <c r="ES23" s="6">
+        <v>1311896</v>
+      </c>
+      <c r="ET23" s="6">
+        <v>760286</v>
+      </c>
+      <c r="EU23" s="6">
+        <v>694155</v>
+      </c>
+      <c r="EV23" s="6">
+        <v>688232</v>
+      </c>
+      <c r="EW23" s="6">
+        <v>199899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -13521,8 +14011,35 @@
       <c r="EG24" s="6">
         <v>34941</v>
       </c>
-    </row>
-    <row r="25" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EO24" t="s">
+        <v>66</v>
+      </c>
+      <c r="EP24" s="6">
+        <v>9183586</v>
+      </c>
+      <c r="EQ24" s="6">
+        <v>7028970</v>
+      </c>
+      <c r="ER24" s="6">
+        <v>4612602</v>
+      </c>
+      <c r="ES24" s="6">
+        <v>5080256</v>
+      </c>
+      <c r="ET24" s="6">
+        <v>4756162</v>
+      </c>
+      <c r="EU24" s="6">
+        <v>6102068</v>
+      </c>
+      <c r="EV24" s="6">
+        <v>4600744</v>
+      </c>
+      <c r="EW24" s="6">
+        <v>4185836</v>
+      </c>
+    </row>
+    <row r="25" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -13637,8 +14154,35 @@
       <c r="BO25" s="6">
         <v>542443</v>
       </c>
-    </row>
-    <row r="26" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EO25" t="s">
+        <v>67</v>
+      </c>
+      <c r="EP25" s="6">
+        <v>9149197</v>
+      </c>
+      <c r="EQ25" s="6">
+        <v>6826197</v>
+      </c>
+      <c r="ER25" s="6">
+        <v>4542780</v>
+      </c>
+      <c r="ES25" s="6">
+        <v>1875650</v>
+      </c>
+      <c r="ET25" s="6">
+        <v>755034</v>
+      </c>
+      <c r="EU25" s="6">
+        <v>739376</v>
+      </c>
+      <c r="EV25" s="6">
+        <v>741477</v>
+      </c>
+      <c r="EW25" s="6">
+        <v>218215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -13779,7 +14323,7 @@
       <c r="DC26" s="6"/>
       <c r="DD26" s="6"/>
     </row>
-    <row r="27" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -13981,7 +14525,7 @@
       </c>
       <c r="DG27" s="9"/>
     </row>
-    <row r="28" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -14190,7 +14734,7 @@
       </c>
       <c r="DG28" s="9"/>
     </row>
-    <row r="29" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -14380,8 +14924,38 @@
         <v>2</v>
       </c>
       <c r="DG29" s="9"/>
-    </row>
-    <row r="30" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EO29" t="s">
+        <v>15</v>
+      </c>
+      <c r="EP29" s="16">
+        <v>2389937173793</v>
+      </c>
+      <c r="EQ29" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="ER29" s="9"/>
+      <c r="ES29" t="s">
+        <v>17</v>
+      </c>
+      <c r="ET29" s="16">
+        <v>646032858217</v>
+      </c>
+      <c r="EU29" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="EV29" s="9"/>
+      <c r="EW29" t="s">
+        <v>29</v>
+      </c>
+      <c r="EX29" s="16">
+        <v>2296395260793</v>
+      </c>
+      <c r="EY29" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="EZ29" s="9"/>
+    </row>
+    <row r="30" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>98</v>
       </c>
@@ -14556,8 +15130,29 @@
         <f>DE30/DE29*100</f>
         <v>56.337958122489162</v>
       </c>
-    </row>
-    <row r="31" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP30" s="16">
+        <v>660804376770</v>
+      </c>
+      <c r="EQ30" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="ER30" s="9"/>
+      <c r="ET30" s="16">
+        <v>124957595207</v>
+      </c>
+      <c r="EU30" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="EV30" s="9"/>
+      <c r="EX30" s="16">
+        <v>169391314794</v>
+      </c>
+      <c r="EY30" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="EZ30" s="9"/>
+    </row>
+    <row r="31" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>99</v>
       </c>
@@ -14765,8 +15360,29 @@
         <v>0</v>
       </c>
       <c r="EJ31" s="9"/>
-    </row>
-    <row r="32" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP31" s="17">
+        <v>606632847</v>
+      </c>
+      <c r="EQ31" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="ER31" s="9"/>
+      <c r="ET31" s="17">
+        <v>283599689</v>
+      </c>
+      <c r="EU31" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="EV31" s="9"/>
+      <c r="EX31" s="17">
+        <v>645543781</v>
+      </c>
+      <c r="EY31" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="EZ31" s="9"/>
+    </row>
+    <row r="32" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -14958,8 +15574,38 @@
         <v>1</v>
       </c>
       <c r="EJ32" s="9"/>
-    </row>
-    <row r="33" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP32" s="17">
+        <v>294143528</v>
+      </c>
+      <c r="EQ32" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="ER32" s="6">
+        <f>EP32/EP31*100</f>
+        <v>48.487899963649674</v>
+      </c>
+      <c r="ET32" s="17">
+        <v>108152592</v>
+      </c>
+      <c r="EU32" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="EV32" s="6">
+        <f>ET32/ET31*100</f>
+        <v>38.135652539449715</v>
+      </c>
+      <c r="EX32" s="17">
+        <v>277100579</v>
+      </c>
+      <c r="EY32" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="EZ32" s="6">
+        <f>EX32/EX31*100</f>
+        <v>42.925141122225455</v>
+      </c>
+    </row>
+    <row r="33" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -15134,8 +15780,29 @@
         <v>2</v>
       </c>
       <c r="EJ33" s="9"/>
-    </row>
-    <row r="34" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP33" s="16">
+        <v>224017281221</v>
+      </c>
+      <c r="EQ33" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="ER33" s="6"/>
+      <c r="ET33" s="16">
+        <v>39077399087</v>
+      </c>
+      <c r="EU33" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="EV33" s="6"/>
+      <c r="EX33" s="16">
+        <v>58603782241</v>
+      </c>
+      <c r="EY33" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="EZ33" s="6"/>
+    </row>
+    <row r="34" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -15186,19 +15853,19 @@
       <c r="AG34" t="s">
         <v>175</v>
       </c>
-      <c r="AH34" s="17">
+      <c r="AH34" s="16">
         <v>87977644370</v>
       </c>
-      <c r="AI34" s="18">
+      <c r="AI34" s="17">
         <v>15105354</v>
       </c>
-      <c r="AJ34" s="18">
+      <c r="AJ34" s="17">
         <v>6953006</v>
       </c>
-      <c r="AK34" s="17">
+      <c r="AK34" s="16">
         <v>55506693569</v>
       </c>
-      <c r="AL34" s="17">
+      <c r="AL34" s="16">
         <v>40131916244</v>
       </c>
       <c r="AU34" s="9">
@@ -15330,8 +15997,38 @@
         <f>EH34/EH33*100</f>
         <v>85.248919293885777</v>
       </c>
-    </row>
-    <row r="35" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP34" s="17">
+        <v>58822021</v>
+      </c>
+      <c r="EQ34" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="ER34" s="6">
+        <f>EP34/EP33*100</f>
+        <v>2.6257805058338444E-2</v>
+      </c>
+      <c r="ET34" s="17">
+        <v>32678501</v>
+      </c>
+      <c r="EU34" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="EV34" s="6">
+        <f>ET34/ET33*100</f>
+        <v>8.3625066569159814E-2</v>
+      </c>
+      <c r="EX34" s="17">
+        <v>61852540</v>
+      </c>
+      <c r="EY34" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="EZ34" s="6">
+        <f>EX34/EX33*100</f>
+        <v>0.10554359741772285</v>
+      </c>
+    </row>
+    <row r="35" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -15374,19 +16071,19 @@
       <c r="AG35" t="s">
         <v>176</v>
       </c>
-      <c r="AH35" s="17">
+      <c r="AH35" s="16">
         <v>2688126327095</v>
       </c>
-      <c r="AI35" s="18">
+      <c r="AI35" s="17">
         <v>270048446</v>
       </c>
-      <c r="AJ35" s="18">
+      <c r="AJ35" s="17">
         <v>218307168</v>
       </c>
-      <c r="AK35" s="17">
+      <c r="AK35" s="16">
         <v>2671171889988</v>
       </c>
-      <c r="AL35" s="17">
+      <c r="AL35" s="16">
         <v>2610227320872</v>
       </c>
       <c r="AU35" s="9">
@@ -15500,8 +16197,29 @@
         <v>4</v>
       </c>
       <c r="EJ35" s="6"/>
-    </row>
-    <row r="36" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP35" s="16">
+        <v>152919551428</v>
+      </c>
+      <c r="EQ35" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="ER35" s="6"/>
+      <c r="ET35" s="16">
+        <v>72912015225</v>
+      </c>
+      <c r="EU35" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="EV35" s="6"/>
+      <c r="EX35" s="16">
+        <v>147703485104</v>
+      </c>
+      <c r="EY35" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="EZ35" s="6"/>
+    </row>
+    <row r="36" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -15544,19 +16262,19 @@
       <c r="AG36" t="s">
         <v>177</v>
       </c>
-      <c r="AH36" s="17">
+      <c r="AH36" s="16">
         <v>76350218497</v>
       </c>
-      <c r="AI36" s="18">
+      <c r="AI36" s="17">
         <v>14299233</v>
       </c>
-      <c r="AJ36" s="18">
+      <c r="AJ36" s="17">
         <v>6472880</v>
       </c>
-      <c r="AK36" s="17">
+      <c r="AK36" s="16">
         <v>46513897591</v>
       </c>
-      <c r="AL36" s="17">
+      <c r="AL36" s="16">
         <v>34748097425</v>
       </c>
       <c r="AU36" s="9">
@@ -15697,8 +16415,29 @@
         <f>EH36/EH35*100</f>
         <v>0.13752912753557778</v>
       </c>
-    </row>
-    <row r="37" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP36" s="17">
+        <v>1156637.2533209999</v>
+      </c>
+      <c r="EQ36" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="ER36" s="6"/>
+      <c r="ET36" s="17">
+        <v>554405.42985399999</v>
+      </c>
+      <c r="EU36" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="EV36" s="6"/>
+      <c r="EX36" s="17">
+        <v>1117854.2708759999</v>
+      </c>
+      <c r="EY36" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="EZ36" s="6"/>
+    </row>
+    <row r="37" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>105</v>
       </c>
@@ -15840,8 +16579,29 @@
         <v>6</v>
       </c>
       <c r="EJ37" s="6"/>
-    </row>
-    <row r="38" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP37" s="17">
+        <v>1156616.39362</v>
+      </c>
+      <c r="EQ37" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="ER37" s="6"/>
+      <c r="ET37" s="17">
+        <v>554395.72138200002</v>
+      </c>
+      <c r="EU37" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="EV37" s="6"/>
+      <c r="EX37" s="17">
+        <v>1117842.0291820001</v>
+      </c>
+      <c r="EY37" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="EZ37" s="6"/>
+    </row>
+    <row r="38" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>106</v>
       </c>
@@ -15963,8 +16723,38 @@
         <v>7</v>
       </c>
       <c r="EJ38" s="6"/>
-    </row>
-    <row r="39" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP38" s="16">
+        <v>1964036807307</v>
+      </c>
+      <c r="EQ38" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="ER38" s="6">
+        <f>EP38/EP29*100</f>
+        <v>82.17943253252696</v>
+      </c>
+      <c r="ET38" s="16">
+        <v>579029355733</v>
+      </c>
+      <c r="EU38" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="EV38" s="6">
+        <f>ET38/ET29*100</f>
+        <v>89.62846833070931</v>
+      </c>
+      <c r="EX38" s="16">
+        <v>2198125025550</v>
+      </c>
+      <c r="EY38" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="EZ38" s="6">
+        <f>EX38/EX29*100</f>
+        <v>95.720674183543437</v>
+      </c>
+    </row>
+    <row r="39" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -16056,8 +16846,38 @@
         <v>8</v>
       </c>
       <c r="EJ39" s="6"/>
-    </row>
-    <row r="40" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EP39" s="16">
+        <v>1093769642564</v>
+      </c>
+      <c r="EQ39" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="ER39" s="6">
+        <f>EP39/EP29*100</f>
+        <v>45.765623237204593</v>
+      </c>
+      <c r="ET39" s="16">
+        <v>354762671002</v>
+      </c>
+      <c r="EU39" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="EV39" s="6">
+        <f>ET39/ET29*100</f>
+        <v>54.914028983156847</v>
+      </c>
+      <c r="EX39" s="16">
+        <v>1304107137324</v>
+      </c>
+      <c r="EY39" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="EZ39" s="6">
+        <f>EX39/EX29*100</f>
+        <v>56.789314957637593</v>
+      </c>
+    </row>
+    <row r="40" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -16172,7 +16992,7 @@
         <v>99.270740718649037</v>
       </c>
     </row>
-    <row r="41" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:156" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -16202,31 +17022,31 @@
       <c r="AT41" t="s">
         <v>175</v>
       </c>
-      <c r="AU41" s="17">
+      <c r="AU41" s="16">
         <v>2328498915018</v>
       </c>
-      <c r="AV41" s="17">
+      <c r="AV41" s="16">
         <v>2209025091912</v>
       </c>
-      <c r="AW41" s="17">
+      <c r="AW41" s="16">
         <v>1323893108298</v>
       </c>
       <c r="CV41" t="s">
         <v>177</v>
       </c>
-      <c r="CW41" s="17">
+      <c r="CW41" s="16">
         <v>76350218497</v>
       </c>
-      <c r="CX41" s="17">
+      <c r="CX41" s="16">
         <v>13956670084</v>
       </c>
-      <c r="CY41" s="18">
+      <c r="CY41" s="17">
         <v>1592379</v>
       </c>
-      <c r="CZ41" s="17">
+      <c r="CZ41" s="16">
         <v>46513897591</v>
       </c>
-      <c r="DA41" s="17">
+      <c r="DA41" s="16">
         <v>34748097425</v>
       </c>
       <c r="DC41" s="6"/>
@@ -16291,19 +17111,34 @@
         <f>EH41/EH31*100</f>
         <v>92.601434594330428</v>
       </c>
-    </row>
-    <row r="42" spans="1:140" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="EP41" t="s">
+        <v>178</v>
+      </c>
+      <c r="EQ41" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="ER41" t="s">
+        <v>189</v>
+      </c>
+      <c r="ES41" t="s">
+        <v>181</v>
+      </c>
+      <c r="ET41" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-      <c r="I42" s="16"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
       <c r="W42" s="6">
         <v>823899138339</v>
       </c>
@@ -16319,38 +17154,56 @@
       <c r="AT42" t="s">
         <v>176</v>
       </c>
-      <c r="AU42" s="17">
+      <c r="AU42" s="16">
         <v>133079155737</v>
       </c>
-      <c r="AV42" s="17">
+      <c r="AV42" s="16">
         <v>99528869971</v>
       </c>
-      <c r="AW42" s="17">
+      <c r="AW42" s="16">
         <v>65633478739</v>
       </c>
       <c r="CV42" t="s">
         <v>197</v>
       </c>
-      <c r="CW42" s="17">
+      <c r="CW42" s="16">
         <v>1955671513701</v>
       </c>
-      <c r="CX42" s="17">
+      <c r="CX42" s="16">
         <v>94298549602</v>
       </c>
-      <c r="CY42" s="18">
+      <c r="CY42" s="17">
         <v>59932069</v>
       </c>
-      <c r="CZ42" s="17">
+      <c r="CZ42" s="16">
         <v>1769874188963</v>
       </c>
-      <c r="DA42" s="17">
+      <c r="DA42" s="16">
         <v>639782428514</v>
       </c>
       <c r="DC42" s="6"/>
       <c r="DD42" s="9"/>
       <c r="DP42" s="6"/>
-    </row>
-    <row r="43" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EO42" t="s">
+        <v>177</v>
+      </c>
+      <c r="EP42" s="16">
+        <v>2389937173793</v>
+      </c>
+      <c r="EQ42" s="16">
+        <v>224017281221</v>
+      </c>
+      <c r="ER42" s="17">
+        <v>58822021</v>
+      </c>
+      <c r="ES42" s="16">
+        <v>1964036807307</v>
+      </c>
+      <c r="ET42" s="16">
+        <v>1093769642564</v>
+      </c>
+    </row>
+    <row r="43" spans="1:156" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>1</v>
       </c>
@@ -16390,37 +17243,55 @@
       <c r="AT43" t="s">
         <v>177</v>
       </c>
-      <c r="AU43" s="17">
+      <c r="AU43" s="16">
         <v>2389937173793</v>
       </c>
-      <c r="AV43" s="17">
+      <c r="AV43" s="16">
         <v>1964036807307</v>
       </c>
-      <c r="AW43" s="17">
+      <c r="AW43" s="16">
         <v>1093769642564</v>
       </c>
       <c r="CV43" t="s">
         <v>198</v>
       </c>
-      <c r="CW43" s="17">
+      <c r="CW43" s="16">
         <v>2392193598736</v>
       </c>
-      <c r="CX43" s="17">
+      <c r="CX43" s="16">
         <v>24723182897</v>
       </c>
-      <c r="CY43" s="18">
+      <c r="CY43" s="17">
         <v>43365885</v>
       </c>
-      <c r="CZ43" s="17">
+      <c r="CZ43" s="16">
         <v>2334013411706</v>
       </c>
-      <c r="DA43" s="17">
+      <c r="DA43" s="16">
         <v>2148763530540</v>
       </c>
       <c r="DC43" s="6"/>
       <c r="DD43" s="9"/>
-    </row>
-    <row r="44" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EO43" t="s">
+        <v>197</v>
+      </c>
+      <c r="EP43" s="16">
+        <v>646032858217</v>
+      </c>
+      <c r="EQ43" s="16">
+        <v>39077399087</v>
+      </c>
+      <c r="ER43" s="17">
+        <v>32678501</v>
+      </c>
+      <c r="ES43" s="16">
+        <v>579029355733</v>
+      </c>
+      <c r="ET43" s="16">
+        <v>354762671002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -16488,8 +17359,26 @@
       <c r="ED44" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="45" spans="1:140" x14ac:dyDescent="0.25">
+      <c r="EO44" t="s">
+        <v>198</v>
+      </c>
+      <c r="EP44" s="16">
+        <v>2296395260793</v>
+      </c>
+      <c r="EQ44" s="16">
+        <v>58603782241</v>
+      </c>
+      <c r="ER44" s="17">
+        <v>61852540</v>
+      </c>
+      <c r="ES44" s="16">
+        <v>2198125025550</v>
+      </c>
+      <c r="ET44" s="16">
+        <v>1304107137324</v>
+      </c>
+    </row>
+    <row r="45" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -16537,23 +17426,23 @@
       <c r="DY45" t="s">
         <v>176</v>
       </c>
-      <c r="DZ45" s="17">
+      <c r="DZ45" s="16">
         <v>89166484910</v>
       </c>
-      <c r="EA45" s="18">
+      <c r="EA45" s="17">
         <v>29327638</v>
       </c>
-      <c r="EB45" s="18">
+      <c r="EB45" s="17">
         <v>17274612</v>
       </c>
-      <c r="EC45" s="17">
+      <c r="EC45" s="16">
         <v>53053893924</v>
       </c>
-      <c r="ED45" s="17">
+      <c r="ED45" s="16">
         <v>41094577766</v>
       </c>
     </row>
-    <row r="46" spans="1:140" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -16609,23 +17498,23 @@
       <c r="DY46" t="s">
         <v>200</v>
       </c>
-      <c r="DZ46" s="17">
+      <c r="DZ46" s="16">
         <v>2674885047666</v>
       </c>
-      <c r="EA46" s="18">
+      <c r="EA46" s="17">
         <v>350873771</v>
       </c>
-      <c r="EB46" s="18">
+      <c r="EB46" s="17">
         <v>283596432</v>
       </c>
-      <c r="EC46" s="17">
+      <c r="EC46" s="16">
         <v>2658391743548</v>
       </c>
-      <c r="ED46" s="17">
+      <c r="ED46" s="16">
         <v>2601322552277</v>
       </c>
     </row>
-    <row r="47" spans="1:140" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:156" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -16680,23 +17569,23 @@
       <c r="DY47" t="s">
         <v>201</v>
       </c>
-      <c r="DZ47" s="17">
+      <c r="DZ47" s="16">
         <v>2687656709105</v>
       </c>
-      <c r="EA47" s="18">
+      <c r="EA47" s="17">
         <v>235207099</v>
       </c>
-      <c r="EB47" s="18">
+      <c r="EB47" s="17">
         <v>200511510</v>
       </c>
-      <c r="EC47" s="17">
+      <c r="EC47" s="16">
         <v>2668056723103</v>
       </c>
-      <c r="ED47" s="17">
+      <c r="ED47" s="16">
         <v>2488808669602</v>
       </c>
     </row>
-    <row r="48" spans="1:140" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:156" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -18636,17 +19525,17 @@
       </c>
     </row>
     <row r="83" spans="1:95" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
+      <c r="A83" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B83" s="16"/>
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
-      <c r="G83" s="16"/>
-      <c r="H83" s="16"/>
-      <c r="I83" s="16"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
       <c r="W83" s="6">
         <v>187767020196</v>
       </c>
@@ -19278,17 +20167,17 @@
       </c>
     </row>
     <row r="91" spans="1:95" x14ac:dyDescent="0.25">
-      <c r="A91" s="16" t="s">
+      <c r="A91" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B91" s="16"/>
-      <c r="C91" s="16"/>
-      <c r="D91" s="16"/>
-      <c r="E91" s="16"/>
-      <c r="F91" s="16"/>
-      <c r="G91" s="16"/>
-      <c r="H91" s="16"/>
-      <c r="I91" s="16"/>
+      <c r="B91" s="18"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="18"/>
+      <c r="F91" s="18"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
       <c r="L91" s="1"/>
       <c r="W91" s="6">
         <v>45260435</v>
@@ -19392,19 +20281,19 @@
       <c r="BG93" t="s">
         <v>185</v>
       </c>
-      <c r="BH93" s="17">
+      <c r="BH93" s="16">
         <v>87977644370</v>
       </c>
-      <c r="BI93" s="18">
+      <c r="BI93" s="17">
         <v>15105354</v>
       </c>
-      <c r="BJ93" s="18">
+      <c r="BJ93" s="17">
         <v>6953006</v>
       </c>
-      <c r="BK93" s="17">
+      <c r="BK93" s="16">
         <v>15685305556</v>
       </c>
-      <c r="BL93" s="18">
+      <c r="BL93" s="17">
         <v>1668487</v>
       </c>
     </row>
@@ -19443,19 +20332,19 @@
       <c r="BG94" t="s">
         <v>186</v>
       </c>
-      <c r="BH94" s="17">
+      <c r="BH94" s="16">
         <v>2328498915018</v>
       </c>
-      <c r="BI94" s="18">
+      <c r="BI94" s="17">
         <v>586732296</v>
       </c>
-      <c r="BJ94" s="18">
+      <c r="BJ94" s="17">
         <v>278268052</v>
       </c>
-      <c r="BK94" s="17">
+      <c r="BK94" s="16">
         <v>75344438595</v>
       </c>
-      <c r="BL94" s="18">
+      <c r="BL94" s="17">
         <v>53676585</v>
       </c>
     </row>
@@ -19478,19 +20367,19 @@
       <c r="BG95" t="s">
         <v>187</v>
       </c>
-      <c r="BH95" s="17">
+      <c r="BH95" s="16">
         <v>2215804132404</v>
       </c>
-      <c r="BI95" s="18">
+      <c r="BI95" s="17">
         <v>620966784</v>
       </c>
-      <c r="BJ95" s="18">
+      <c r="BJ95" s="17">
         <v>248194517</v>
       </c>
-      <c r="BK95" s="17">
+      <c r="BK95" s="16">
         <v>60859222000</v>
       </c>
-      <c r="BL95" s="18">
+      <c r="BL95" s="17">
         <v>58042275</v>
       </c>
     </row>
@@ -19555,17 +20444,17 @@
       </c>
     </row>
     <row r="99" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A99" s="16" t="s">
+      <c r="A99" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B99" s="16"/>
-      <c r="C99" s="16"/>
-      <c r="D99" s="16"/>
-      <c r="E99" s="16"/>
-      <c r="F99" s="16"/>
-      <c r="G99" s="16"/>
-      <c r="H99" s="16"/>
-      <c r="I99" s="16"/>
+      <c r="B99" s="18"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18"/>
+      <c r="G99" s="18"/>
+      <c r="H99" s="18"/>
+      <c r="I99" s="18"/>
       <c r="W99" s="6">
         <v>6995467846</v>
       </c>
@@ -19717,15 +20606,15 @@
       </c>
     </row>
     <row r="105" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A105" s="16"/>
-      <c r="B105" s="16"/>
-      <c r="C105" s="16"/>
-      <c r="D105" s="16"/>
-      <c r="E105" s="16"/>
-      <c r="F105" s="16"/>
-      <c r="G105" s="16"/>
-      <c r="H105" s="16"/>
-      <c r="I105" s="16"/>
+      <c r="A105" s="18"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18"/>
+      <c r="I105" s="18"/>
       <c r="W105" s="6">
         <v>230536003706</v>
       </c>
@@ -19740,17 +20629,17 @@
       </c>
     </row>
     <row r="106" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A106" s="16" t="s">
+      <c r="A106" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="B106" s="16"/>
-      <c r="C106" s="16"/>
-      <c r="D106" s="16"/>
-      <c r="E106" s="16"/>
-      <c r="F106" s="16"/>
-      <c r="G106" s="16"/>
-      <c r="H106" s="16"/>
-      <c r="I106" s="16"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
+      <c r="E106" s="18"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
       <c r="L106" s="1"/>
       <c r="W106" s="6">
         <v>35974891</v>
@@ -20376,17 +21265,17 @@
       </c>
     </row>
     <row r="122" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A122" s="16" t="s">
+      <c r="A122" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="B122" s="16"/>
-      <c r="C122" s="16"/>
-      <c r="D122" s="16"/>
-      <c r="E122" s="16"/>
-      <c r="F122" s="16"/>
-      <c r="G122" s="16"/>
-      <c r="H122" s="16"/>
-      <c r="I122" s="16"/>
+      <c r="B122" s="18"/>
+      <c r="C122" s="18"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="18"/>
+      <c r="F122" s="18"/>
+      <c r="G122" s="18"/>
+      <c r="H122" s="18"/>
+      <c r="I122" s="18"/>
       <c r="J122" s="8"/>
       <c r="W122" s="6">
         <v>58912066564</v>
@@ -25216,13 +26105,6 @@
       <c r="K260" s="1"/>
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J261" s="6">
-        <v>2296395260793</v>
-      </c>
-      <c r="K261" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="L261" s="9"/>
       <c r="M261" t="s">
         <v>32</v>
       </c>
@@ -25255,16 +26137,6 @@
         <v>0</v>
       </c>
       <c r="H262" s="9"/>
-      <c r="I262" t="s">
-        <v>29</v>
-      </c>
-      <c r="J262" s="6">
-        <v>169391314794</v>
-      </c>
-      <c r="K262" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="L262" s="9"/>
       <c r="N262" s="6">
         <v>93217588295</v>
       </c>
@@ -25288,13 +26160,6 @@
         <v>1</v>
       </c>
       <c r="H263" s="9"/>
-      <c r="J263" s="6">
-        <v>645543781</v>
-      </c>
-      <c r="K263" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="L263" s="9"/>
       <c r="N263" s="6">
         <v>397342891</v>
       </c>
@@ -25318,16 +26183,6 @@
         <v>2</v>
       </c>
       <c r="H264" s="9"/>
-      <c r="J264" s="6">
-        <v>277100579</v>
-      </c>
-      <c r="K264" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="L264" s="6">
-        <f>J264/J263*100</f>
-        <v>42.925141122225455</v>
-      </c>
       <c r="N264" s="6">
         <v>139760813</v>
       </c>
@@ -25360,13 +26215,6 @@
         <f>F265/F264*100</f>
         <v>44.733752856289449</v>
       </c>
-      <c r="J265" s="6">
-        <v>58603782241</v>
-      </c>
-      <c r="K265" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="L265" s="6"/>
       <c r="N265" s="6">
         <v>23211224675</v>
       </c>
@@ -25390,16 +26238,6 @@
         <v>4</v>
       </c>
       <c r="H266" s="6"/>
-      <c r="J266" s="6">
-        <v>61852540</v>
-      </c>
-      <c r="K266" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L266" s="6">
-        <f>J266/J265*100</f>
-        <v>0.10554359741772285</v>
-      </c>
       <c r="N266" s="6">
         <v>55423868</v>
       </c>
@@ -25432,13 +26270,6 @@
         <f>F267/F266*100</f>
         <v>0.7134941620396853</v>
       </c>
-      <c r="J267" s="6">
-        <v>147703485104</v>
-      </c>
-      <c r="K267" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L267" s="6"/>
       <c r="N267" s="6">
         <v>15016386180</v>
       </c>
@@ -25462,13 +26293,6 @@
         <v>6</v>
       </c>
       <c r="H268" s="6"/>
-      <c r="J268" s="6">
-        <v>1117854.2708759999</v>
-      </c>
-      <c r="K268" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="L268" s="6"/>
       <c r="N268" s="6">
         <v>117410.55757200001</v>
       </c>
@@ -25492,13 +26316,6 @@
         <v>7</v>
       </c>
       <c r="H269" s="6"/>
-      <c r="J269" s="6">
-        <v>1117842.0291820001</v>
-      </c>
-      <c r="K269" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L269" s="6"/>
       <c r="N269" s="6">
         <v>117409.079065</v>
       </c>
@@ -25522,16 +26339,6 @@
         <v>8</v>
       </c>
       <c r="H270" s="6"/>
-      <c r="J270" s="6">
-        <v>2198125025550</v>
-      </c>
-      <c r="K270" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="L270" s="6">
-        <f>J270/J261*100</f>
-        <v>95.720674183543437</v>
-      </c>
       <c r="N270" s="6">
         <v>164986920068</v>
       </c>
@@ -25563,16 +26370,6 @@
       <c r="H271" s="6">
         <f>F271/F262*100</f>
         <v>89.69121496533468</v>
-      </c>
-      <c r="J271" s="6">
-        <v>1304107137324</v>
-      </c>
-      <c r="K271" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L271" s="6">
-        <f>J271/J261*100</f>
-        <v>56.789314957637593</v>
       </c>
       <c r="N271" s="6">
         <v>106636223668</v>
@@ -28185,16 +28982,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K4:S4"/>
+    <mergeCell ref="K19:S19"/>
+    <mergeCell ref="A106:I106"/>
+    <mergeCell ref="A122:I122"/>
+    <mergeCell ref="A105:I105"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A83:I83"/>
     <mergeCell ref="A91:I91"/>
     <mergeCell ref="A99:I99"/>
     <mergeCell ref="A42:I42"/>
-    <mergeCell ref="K4:S4"/>
-    <mergeCell ref="K19:S19"/>
-    <mergeCell ref="A106:I106"/>
-    <mergeCell ref="A122:I122"/>
-    <mergeCell ref="A105:I105"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished the report, now making minor changes as I proofread
</commit_message>
<xml_diff>
--- a/Data Structures/hash_table/hash_table_data.xlsx
+++ b/Data Structures/hash_table/hash_table_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="202">
   <si>
     <t>cycles</t>
   </si>
@@ -1100,11 +1100,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99128448"/>
-        <c:axId val="99130368"/>
+        <c:axId val="101618816"/>
+        <c:axId val="101620736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99128448"/>
+        <c:axId val="101618816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,7 +1133,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99130368"/>
+        <c:crossAx val="101620736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1141,7 +1141,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99130368"/>
+        <c:axId val="101620736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,7 +1171,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99128448"/>
+        <c:crossAx val="101618816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1501,11 +1501,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107697664"/>
-        <c:axId val="107699584"/>
+        <c:axId val="113063424"/>
+        <c:axId val="113065344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107697664"/>
+        <c:axId val="113063424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1534,7 +1534,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107699584"/>
+        <c:crossAx val="113065344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1542,7 +1542,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107699584"/>
+        <c:axId val="113065344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,7 +1572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107697664"/>
+        <c:crossAx val="113063424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1820,11 +1820,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107721472"/>
-        <c:axId val="107723392"/>
+        <c:axId val="113087232"/>
+        <c:axId val="113089152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107721472"/>
+        <c:axId val="113087232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1853,7 +1853,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107723392"/>
+        <c:crossAx val="113089152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1861,7 +1861,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107723392"/>
+        <c:axId val="113089152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1891,7 +1891,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107721472"/>
+        <c:crossAx val="113087232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2142,11 +2142,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107835776"/>
-        <c:axId val="107837696"/>
+        <c:axId val="113140096"/>
+        <c:axId val="113142016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107835776"/>
+        <c:axId val="113140096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2175,7 +2175,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107837696"/>
+        <c:crossAx val="113142016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2183,7 +2183,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107837696"/>
+        <c:axId val="113142016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,7 +2213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107835776"/>
+        <c:crossAx val="113140096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2546,11 +2546,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107938560"/>
-        <c:axId val="107940480"/>
+        <c:axId val="113251072"/>
+        <c:axId val="113252992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107938560"/>
+        <c:axId val="113251072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2579,7 +2579,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107940480"/>
+        <c:crossAx val="113252992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2587,7 +2587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107940480"/>
+        <c:axId val="113252992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2617,7 +2617,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107938560"/>
+        <c:crossAx val="113251072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2950,11 +2950,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107996288"/>
-        <c:axId val="107998208"/>
+        <c:axId val="113304704"/>
+        <c:axId val="113306624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107996288"/>
+        <c:axId val="113304704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2983,7 +2983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107998208"/>
+        <c:crossAx val="113306624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2991,7 +2991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107998208"/>
+        <c:axId val="113306624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3021,7 +3021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107996288"/>
+        <c:crossAx val="113304704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -3354,11 +3354,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108037632"/>
-        <c:axId val="108039552"/>
+        <c:axId val="113350144"/>
+        <c:axId val="113352064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108037632"/>
+        <c:axId val="113350144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3387,7 +3387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108039552"/>
+        <c:crossAx val="113352064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3395,7 +3395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108039552"/>
+        <c:axId val="113352064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3413,7 +3413,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>Millions of Iterations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3425,9 +3425,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108037632"/>
+        <c:crossAx val="113350144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3755,11 +3758,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108070784"/>
-        <c:axId val="108077056"/>
+        <c:axId val="113444736"/>
+        <c:axId val="113451008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108070784"/>
+        <c:axId val="113444736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3788,7 +3791,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108077056"/>
+        <c:crossAx val="113451008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3796,7 +3799,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108077056"/>
+        <c:axId val="113451008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3826,7 +3829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108070784"/>
+        <c:crossAx val="113444736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -4159,11 +4162,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108128512"/>
-        <c:axId val="107348352"/>
+        <c:axId val="113506560"/>
+        <c:axId val="113525120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108128512"/>
+        <c:axId val="113506560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4192,7 +4195,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107348352"/>
+        <c:crossAx val="113525120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4200,7 +4203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107348352"/>
+        <c:axId val="113525120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4230,7 +4233,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108128512"/>
+        <c:crossAx val="113506560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4560,11 +4563,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107383040"/>
-        <c:axId val="107405696"/>
+        <c:axId val="113551616"/>
+        <c:axId val="113566080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107383040"/>
+        <c:axId val="113551616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4593,7 +4596,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107405696"/>
+        <c:crossAx val="113566080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4601,7 +4604,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107405696"/>
+        <c:axId val="113566080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4631,7 +4634,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107383040"/>
+        <c:crossAx val="113551616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -4964,11 +4967,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107485824"/>
-        <c:axId val="107492096"/>
+        <c:axId val="113592960"/>
+        <c:axId val="113599232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107485824"/>
+        <c:axId val="113592960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4997,7 +5000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107492096"/>
+        <c:crossAx val="113599232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5005,7 +5008,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107492096"/>
+        <c:axId val="113599232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5035,7 +5038,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107485824"/>
+        <c:crossAx val="113592960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5369,11 +5372,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99320960"/>
-        <c:axId val="99322880"/>
+        <c:axId val="106792064"/>
+        <c:axId val="106793984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99320960"/>
+        <c:axId val="106792064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5402,7 +5405,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99322880"/>
+        <c:crossAx val="106793984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5410,7 +5413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99322880"/>
+        <c:axId val="106793984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5440,7 +5443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99320960"/>
+        <c:crossAx val="106792064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5770,11 +5773,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107523072"/>
-        <c:axId val="107529344"/>
+        <c:axId val="113613824"/>
+        <c:axId val="113620096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107523072"/>
+        <c:axId val="113613824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5803,7 +5806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107529344"/>
+        <c:crossAx val="113620096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5811,7 +5814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107529344"/>
+        <c:axId val="113620096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5841,7 +5844,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107523072"/>
+        <c:crossAx val="113613824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -6174,11 +6177,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113413504"/>
-        <c:axId val="113415680"/>
+        <c:axId val="112762240"/>
+        <c:axId val="112764416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113413504"/>
+        <c:axId val="112762240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6207,7 +6210,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113415680"/>
+        <c:crossAx val="112764416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6215,7 +6218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113415680"/>
+        <c:axId val="112764416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6245,7 +6248,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113413504"/>
+        <c:crossAx val="112762240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -6496,11 +6499,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113716224"/>
-        <c:axId val="113726592"/>
+        <c:axId val="112872448"/>
+        <c:axId val="112878720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113716224"/>
+        <c:axId val="112872448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6529,7 +6532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113726592"/>
+        <c:crossAx val="112878720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6537,7 +6540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113726592"/>
+        <c:axId val="112878720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6567,7 +6570,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113716224"/>
+        <c:crossAx val="112872448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -6900,11 +6903,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45266048"/>
-        <c:axId val="45267968"/>
+        <c:axId val="112901504"/>
+        <c:axId val="112793088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45266048"/>
+        <c:axId val="112901504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6933,7 +6936,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45267968"/>
+        <c:crossAx val="112793088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6941,7 +6944,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45267968"/>
+        <c:axId val="112793088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6971,7 +6974,742 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45266048"/>
+        <c:crossAx val="112901504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$FI$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Bucket TAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$FJ$24:$FQ$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$FJ$25:$FQ$25</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9222903</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5008198</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5138550</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5369570</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5797952</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4288425</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5349241</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4052818</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$FI$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Bucket TAS No Pause</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$FJ$24:$FQ$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$FJ$26:$FQ$26</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7469810</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5090869</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5742197</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4876768</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>818125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>815600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>808121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>443836</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$FI$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) Bucket TAS_RELAX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$FJ$24:$FQ$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$FJ$27:$FQ$27</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9222833</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7531529</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7271930</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>861688</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>829925</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>863566</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>851305</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>442237</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="48110208"/>
+        <c:axId val="48152960"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="48110208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48152960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="48152960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48110208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Lockless Hash Table;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Stoker</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>; Lockless</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>; Table Size 128</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$FU$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core)128  Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$FV$25:$GC$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$FV$26:$GC$26</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8603162</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10941262</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6114190</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5320471</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1488182</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1429951</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1433241</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1388062</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$FU$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Local (4 Core) 128 Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$FV$25:$GC$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$FV$27:$GC$27</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>15927766</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11000234</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10948047</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10937830</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10946077</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10944978</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10947130</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10939622</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$FU$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cube (16 Core) 128 Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$FV$25:$GC$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$FV$28:$GC$28</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6731606</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11670448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7605257</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7541685</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7629871</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7531565</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9009243</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>8224970</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="70080768"/>
+        <c:axId val="70095616"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="70080768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70095616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="70095616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Millions of Iterations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="70080768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -7518,11 +8256,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107093376"/>
-        <c:axId val="107099264"/>
+        <c:axId val="112471424"/>
+        <c:axId val="112481408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107093376"/>
+        <c:axId val="112471424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7532,7 +8270,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107099264"/>
+        <c:crossAx val="112481408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7540,7 +8278,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107099264"/>
+        <c:axId val="112481408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7551,7 +8289,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107093376"/>
+        <c:crossAx val="112471424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8127,11 +8865,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107133184"/>
-        <c:axId val="107135360"/>
+        <c:axId val="112509696"/>
+        <c:axId val="112511616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107133184"/>
+        <c:axId val="112509696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8160,7 +8898,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107135360"/>
+        <c:crossAx val="112511616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8168,7 +8906,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107135360"/>
+        <c:axId val="112511616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8198,7 +8936,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107133184"/>
+        <c:crossAx val="112509696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8446,11 +9184,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106981632"/>
-        <c:axId val="106983808"/>
+        <c:axId val="112624000"/>
+        <c:axId val="112625920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106981632"/>
+        <c:axId val="112624000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8479,7 +9217,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106983808"/>
+        <c:crossAx val="112625920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8487,7 +9225,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106983808"/>
+        <c:axId val="112625920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8517,7 +9255,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106981632"/>
+        <c:crossAx val="112624000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8847,11 +9585,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107014400"/>
-        <c:axId val="107016576"/>
+        <c:axId val="112654592"/>
+        <c:axId val="112656768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107014400"/>
+        <c:axId val="112654592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8880,7 +9618,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107016576"/>
+        <c:crossAx val="112656768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8888,7 +9626,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107016576"/>
+        <c:axId val="112656768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8918,7 +9656,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107014400"/>
+        <c:crossAx val="112654592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -9251,11 +9989,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107084416"/>
-        <c:axId val="107614976"/>
+        <c:axId val="112710784"/>
+        <c:axId val="112712704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107084416"/>
+        <c:axId val="112710784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9284,7 +10022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107614976"/>
+        <c:crossAx val="112712704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9292,7 +10030,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107614976"/>
+        <c:axId val="112712704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9322,7 +10060,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107084416"/>
+        <c:crossAx val="112710784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -9983,11 +10721,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107663744"/>
-        <c:axId val="107665664"/>
+        <c:axId val="107135360"/>
+        <c:axId val="107137280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107663744"/>
+        <c:axId val="107135360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10016,7 +10754,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107665664"/>
+        <c:crossAx val="107137280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10024,7 +10762,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107665664"/>
+        <c:axId val="107137280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10054,7 +10792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107663744"/>
+        <c:crossAx val="107135360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -10469,11 +11207,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107758720"/>
-        <c:axId val="107760640"/>
+        <c:axId val="113005696"/>
+        <c:axId val="113007616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107758720"/>
+        <c:axId val="113005696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10502,7 +11240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107760640"/>
+        <c:crossAx val="113007616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10510,7 +11248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107760640"/>
+        <c:axId val="113007616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10540,7 +11278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107758720"/>
+        <c:crossAx val="113005696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -11297,6 +12035,68 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>164</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>169</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>174</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>191</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="28" name="Chart 27"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -11587,10 +12387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:EZ468"/>
+  <dimension ref="A3:GC468"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EE13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="EO41" sqref="EO41:ET44"/>
+    <sheetView tabSelected="1" topLeftCell="CA49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="GI39" sqref="GI39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11626,7 +12426,7 @@
     <col min="104" max="104" width="13.42578125" customWidth="1"/>
     <col min="106" max="106" width="19.140625" customWidth="1"/>
     <col min="108" max="108" width="13.42578125" customWidth="1"/>
-    <col min="114" max="114" width="19.28515625" customWidth="1"/>
+    <col min="114" max="114" width="31.28515625" customWidth="1"/>
     <col min="119" max="119" width="20.28515625" customWidth="1"/>
     <col min="123" max="123" width="23.85546875" customWidth="1"/>
     <col min="129" max="129" width="26" customWidth="1"/>
@@ -11635,6 +12435,9 @@
     <col min="145" max="145" width="32" customWidth="1"/>
     <col min="149" max="149" width="17.85546875" customWidth="1"/>
     <col min="153" max="153" width="17" customWidth="1"/>
+    <col min="165" max="165" width="29.5703125" customWidth="1"/>
+    <col min="169" max="169" width="15.85546875" customWidth="1"/>
+    <col min="173" max="173" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
@@ -12604,7 +13407,7 @@
         <v>5841043</v>
       </c>
     </row>
-    <row r="17" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -12705,7 +13508,7 @@
         <v>5669610</v>
       </c>
     </row>
-    <row r="18" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -12746,7 +13549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -12798,7 +13601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -12895,7 +13698,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -13164,7 +13967,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -13474,7 +14277,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -13779,7 +14582,7 @@
         <v>199899</v>
       </c>
     </row>
-    <row r="24" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -14038,8 +14841,32 @@
       <c r="EW24" s="6">
         <v>4185836</v>
       </c>
-    </row>
-    <row r="25" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ24">
+        <v>1</v>
+      </c>
+      <c r="FK24">
+        <v>2</v>
+      </c>
+      <c r="FL24">
+        <v>4</v>
+      </c>
+      <c r="FM24">
+        <v>8</v>
+      </c>
+      <c r="FN24">
+        <v>16</v>
+      </c>
+      <c r="FO24">
+        <v>32</v>
+      </c>
+      <c r="FP24">
+        <v>64</v>
+      </c>
+      <c r="FQ24">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -14181,8 +15008,59 @@
       <c r="EW25" s="6">
         <v>218215</v>
       </c>
-    </row>
-    <row r="26" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FI25" t="s">
+        <v>63</v>
+      </c>
+      <c r="FJ25" s="6">
+        <v>9222903</v>
+      </c>
+      <c r="FK25" s="6">
+        <v>5008198</v>
+      </c>
+      <c r="FL25" s="6">
+        <v>5138550</v>
+      </c>
+      <c r="FM25" s="6">
+        <v>5369570</v>
+      </c>
+      <c r="FN25" s="6">
+        <v>5797952</v>
+      </c>
+      <c r="FO25" s="6">
+        <v>4288425</v>
+      </c>
+      <c r="FP25" s="6">
+        <v>5349241</v>
+      </c>
+      <c r="FQ25" s="6">
+        <v>4052818</v>
+      </c>
+      <c r="FV25">
+        <v>1</v>
+      </c>
+      <c r="FW25">
+        <v>2</v>
+      </c>
+      <c r="FX25">
+        <v>4</v>
+      </c>
+      <c r="FY25">
+        <v>8</v>
+      </c>
+      <c r="FZ25">
+        <v>16</v>
+      </c>
+      <c r="GA25">
+        <v>32</v>
+      </c>
+      <c r="GB25">
+        <v>64</v>
+      </c>
+      <c r="GC25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -14322,8 +15200,62 @@
       <c r="DB26" s="6"/>
       <c r="DC26" s="6"/>
       <c r="DD26" s="6"/>
-    </row>
-    <row r="27" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FI26" t="s">
+        <v>64</v>
+      </c>
+      <c r="FJ26" s="6">
+        <v>7469810</v>
+      </c>
+      <c r="FK26" s="6">
+        <v>5090869</v>
+      </c>
+      <c r="FL26" s="6">
+        <v>5742197</v>
+      </c>
+      <c r="FM26" s="6">
+        <v>4876768</v>
+      </c>
+      <c r="FN26" s="6">
+        <v>818125</v>
+      </c>
+      <c r="FO26" s="6">
+        <v>815600</v>
+      </c>
+      <c r="FP26" s="6">
+        <v>808121</v>
+      </c>
+      <c r="FQ26" s="6">
+        <v>443836</v>
+      </c>
+      <c r="FU26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="FV26" s="7">
+        <v>8603162</v>
+      </c>
+      <c r="FW26" s="7">
+        <v>10941262</v>
+      </c>
+      <c r="FX26" s="7">
+        <v>6114190</v>
+      </c>
+      <c r="FY26" s="7">
+        <v>5320471</v>
+      </c>
+      <c r="FZ26" s="7">
+        <v>1488182</v>
+      </c>
+      <c r="GA26" s="7">
+        <v>1429951</v>
+      </c>
+      <c r="GB26" s="7">
+        <v>1433241</v>
+      </c>
+      <c r="GC26" s="7">
+        <v>1388062</v>
+      </c>
+    </row>
+    <row r="27" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -14524,8 +15456,62 @@
         <v>0</v>
       </c>
       <c r="DG27" s="9"/>
-    </row>
-    <row r="28" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FI27" t="s">
+        <v>70</v>
+      </c>
+      <c r="FJ27" s="6">
+        <v>9222833</v>
+      </c>
+      <c r="FK27" s="6">
+        <v>7531529</v>
+      </c>
+      <c r="FL27" s="6">
+        <v>7271930</v>
+      </c>
+      <c r="FM27" s="6">
+        <v>861688</v>
+      </c>
+      <c r="FN27" s="6">
+        <v>829925</v>
+      </c>
+      <c r="FO27" s="6">
+        <v>863566</v>
+      </c>
+      <c r="FP27" s="6">
+        <v>851305</v>
+      </c>
+      <c r="FQ27" s="6">
+        <v>442237</v>
+      </c>
+      <c r="FU27" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="FV27" s="6">
+        <v>15927766</v>
+      </c>
+      <c r="FW27" s="6">
+        <v>11000234</v>
+      </c>
+      <c r="FX27" s="6">
+        <v>10948047</v>
+      </c>
+      <c r="FY27" s="7">
+        <v>10937830</v>
+      </c>
+      <c r="FZ27" s="6">
+        <v>10946077</v>
+      </c>
+      <c r="GA27" s="6">
+        <v>10944978</v>
+      </c>
+      <c r="GB27" s="6">
+        <v>10947130</v>
+      </c>
+      <c r="GC27" s="6">
+        <v>10939622</v>
+      </c>
+    </row>
+    <row r="28" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -14733,8 +15719,35 @@
         <v>1</v>
       </c>
       <c r="DG28" s="9"/>
-    </row>
-    <row r="29" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FU28" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="FV28" s="6">
+        <v>6731606</v>
+      </c>
+      <c r="FW28" s="6">
+        <v>11670448</v>
+      </c>
+      <c r="FX28" s="6">
+        <v>7605257</v>
+      </c>
+      <c r="FY28" s="6">
+        <v>7541685</v>
+      </c>
+      <c r="FZ28" s="6">
+        <v>7629871</v>
+      </c>
+      <c r="GA28" s="6">
+        <v>7531565</v>
+      </c>
+      <c r="GB28" s="6">
+        <v>9009243</v>
+      </c>
+      <c r="GC28">
+        <v>8224970</v>
+      </c>
+    </row>
+    <row r="29" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -14955,7 +15968,7 @@
       </c>
       <c r="EZ29" s="9"/>
     </row>
-    <row r="30" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>98</v>
       </c>
@@ -15152,7 +16165,7 @@
       </c>
       <c r="EZ30" s="9"/>
     </row>
-    <row r="31" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>99</v>
       </c>
@@ -15382,7 +16395,7 @@
       </c>
       <c r="EZ31" s="9"/>
     </row>
-    <row r="32" spans="1:156" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:185" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -15604,8 +16617,38 @@
         <f>EX32/EX31*100</f>
         <v>42.925141122225455</v>
       </c>
-    </row>
-    <row r="33" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FI32" t="s">
+        <v>199</v>
+      </c>
+      <c r="FJ32" s="16">
+        <v>133079155737</v>
+      </c>
+      <c r="FK32" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="FL32" s="9"/>
+      <c r="FM32" t="s">
+        <v>25</v>
+      </c>
+      <c r="FN32" s="16">
+        <v>18826403737</v>
+      </c>
+      <c r="FO32" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="FP32" s="9"/>
+      <c r="FQ32" t="s">
+        <v>33</v>
+      </c>
+      <c r="FR32" s="16">
+        <v>2392936011460</v>
+      </c>
+      <c r="FS32" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="FT32" s="9"/>
+    </row>
+    <row r="33" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -15801,8 +16844,30 @@
         <v>4</v>
       </c>
       <c r="EZ33" s="6"/>
-    </row>
-    <row r="34" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ33" s="16">
+        <v>68608676854</v>
+      </c>
+      <c r="FK33" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="FL33" s="9"/>
+      <c r="FN33" s="16">
+        <v>14472739062</v>
+      </c>
+      <c r="FO33" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="FP33" s="9"/>
+      <c r="FQ33" s="3"/>
+      <c r="FR33" s="16">
+        <v>409062544720</v>
+      </c>
+      <c r="FS33" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="FT33" s="9"/>
+    </row>
+    <row r="34" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -16027,8 +17092,29 @@
         <f>EX34/EX33*100</f>
         <v>0.10554359741772285</v>
       </c>
-    </row>
-    <row r="35" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ34" s="17">
+        <v>55662041</v>
+      </c>
+      <c r="FK34" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="FL34" s="9"/>
+      <c r="FN34" s="17">
+        <v>13788146</v>
+      </c>
+      <c r="FO34" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="FP34" s="9"/>
+      <c r="FR34" s="17">
+        <v>499437562</v>
+      </c>
+      <c r="FS34" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="FT34" s="9"/>
+    </row>
+    <row r="35" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -16218,8 +17304,35 @@
         <v>6</v>
       </c>
       <c r="EZ35" s="6"/>
-    </row>
-    <row r="36" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ35" s="17">
+        <v>24795219</v>
+      </c>
+      <c r="FK35" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="FL35" s="6">
+        <v>44.546011167646547</v>
+      </c>
+      <c r="FN35" s="17">
+        <v>4696341</v>
+      </c>
+      <c r="FO35" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="FP35" s="6">
+        <v>34.060714181587578</v>
+      </c>
+      <c r="FR35" s="17">
+        <v>241397897</v>
+      </c>
+      <c r="FS35" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="FT35" s="6">
+        <v>48.333949099327057</v>
+      </c>
+    </row>
+    <row r="36" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -16436,8 +17549,29 @@
         <v>7</v>
       </c>
       <c r="EZ36" s="6"/>
-    </row>
-    <row r="37" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ36" s="16">
+        <v>16319586294</v>
+      </c>
+      <c r="FK36" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="FL36" s="6"/>
+      <c r="FN36" s="16">
+        <v>3408861433</v>
+      </c>
+      <c r="FO36" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="FP36" s="6"/>
+      <c r="FR36" s="16">
+        <v>110953282559</v>
+      </c>
+      <c r="FS36" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="FT36" s="6"/>
+    </row>
+    <row r="37" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>105</v>
       </c>
@@ -16600,8 +17734,35 @@
         <v>8</v>
       </c>
       <c r="EZ37" s="6"/>
-    </row>
-    <row r="38" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ37" s="17">
+        <v>11995001</v>
+      </c>
+      <c r="FK37" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="FL37" s="6">
+        <v>7.3500643851554248E-2</v>
+      </c>
+      <c r="FN37" s="17">
+        <v>2153695</v>
+      </c>
+      <c r="FO37" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="FP37" s="6">
+        <v>6.3179306121123879E-2</v>
+      </c>
+      <c r="FR37" s="17">
+        <v>47340314</v>
+      </c>
+      <c r="FS37" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="FT37" s="6">
+        <v>4.2666889079939152E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>106</v>
       </c>
@@ -16753,8 +17914,29 @@
         <f>EX38/EX29*100</f>
         <v>95.720674183543437</v>
       </c>
-    </row>
-    <row r="39" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ38" s="16">
+        <v>14378231493</v>
+      </c>
+      <c r="FK38" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="FL38" s="6"/>
+      <c r="FN38" s="16">
+        <v>1569202936</v>
+      </c>
+      <c r="FO38" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="FP38" s="6"/>
+      <c r="FR38" s="16">
+        <v>154061563316</v>
+      </c>
+      <c r="FS38" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="FT38" s="6"/>
+    </row>
+    <row r="39" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -16876,8 +18058,29 @@
         <f>EX39/EX29*100</f>
         <v>56.789314957637593</v>
       </c>
-    </row>
-    <row r="40" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ39" s="17">
+        <v>111395.78911100001</v>
+      </c>
+      <c r="FK39" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="FL39" s="6"/>
+      <c r="FN39" s="17">
+        <v>13213.445659999999</v>
+      </c>
+      <c r="FO39" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="FP39" s="6"/>
+      <c r="FR39" s="17">
+        <v>1164827.0688519999</v>
+      </c>
+      <c r="FS39" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="FT39" s="6"/>
+    </row>
+    <row r="40" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -16991,8 +18194,29 @@
         <f>EH40/EH31*100</f>
         <v>99.270740718649037</v>
       </c>
-    </row>
-    <row r="41" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ40" s="17">
+        <v>111394.21202799999</v>
+      </c>
+      <c r="FK40" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="FL40" s="6"/>
+      <c r="FN40" s="17">
+        <v>13213.484871000001</v>
+      </c>
+      <c r="FO40" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="FP40" s="6"/>
+      <c r="FR40" s="17">
+        <v>1164810.888246</v>
+      </c>
+      <c r="FS40" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="FT40" s="6"/>
+    </row>
+    <row r="41" spans="1:176" x14ac:dyDescent="0.25">
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -17126,8 +18350,35 @@
       <c r="ET41" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="42" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ41" s="16">
+        <v>99528869971</v>
+      </c>
+      <c r="FK41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="FL41" s="6">
+        <v>74.789225570152894</v>
+      </c>
+      <c r="FN41" s="16">
+        <v>11887202724</v>
+      </c>
+      <c r="FO41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="FP41" s="6">
+        <v>63.14112291471676</v>
+      </c>
+      <c r="FR41" s="16">
+        <v>2147746588007</v>
+      </c>
+      <c r="FS41" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="FT41" s="6">
+        <v>89.753615546810934</v>
+      </c>
+    </row>
+    <row r="42" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>41</v>
       </c>
@@ -17202,8 +18453,35 @@
       <c r="ET42" s="16">
         <v>1093769642564</v>
       </c>
-    </row>
-    <row r="43" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ42" s="16">
+        <v>65633478739</v>
+      </c>
+      <c r="FK42" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="FL42" s="6">
+        <v>49.319127684210216</v>
+      </c>
+      <c r="FN42" s="16">
+        <v>7778978828</v>
+      </c>
+      <c r="FO42" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="FP42" s="6">
+        <v>41.319515594535879</v>
+      </c>
+      <c r="FR42" s="16">
+        <v>1267188978449</v>
+      </c>
+      <c r="FS42" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="FT42" s="6">
+        <v>52.955405927292261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:176" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>1</v>
       </c>
@@ -17290,8 +18568,9 @@
       <c r="ET43" s="16">
         <v>354762671002</v>
       </c>
-    </row>
-    <row r="44" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FK43" s="1"/>
+    </row>
+    <row r="44" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -17377,8 +18656,23 @@
       <c r="ET44" s="16">
         <v>1304107137324</v>
       </c>
-    </row>
-    <row r="45" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FJ44" t="s">
+        <v>178</v>
+      </c>
+      <c r="FK44" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="FL44" t="s">
+        <v>180</v>
+      </c>
+      <c r="FM44" t="s">
+        <v>181</v>
+      </c>
+      <c r="FN44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -17441,8 +18735,26 @@
       <c r="ED45" s="16">
         <v>41094577766</v>
       </c>
-    </row>
-    <row r="46" spans="1:156" x14ac:dyDescent="0.25">
+      <c r="FI45" t="s">
+        <v>176</v>
+      </c>
+      <c r="FJ45" s="16">
+        <v>18826403737</v>
+      </c>
+      <c r="FK45" s="17">
+        <v>13788146</v>
+      </c>
+      <c r="FL45" s="17">
+        <v>4696341</v>
+      </c>
+      <c r="FM45" s="16">
+        <v>11887202724</v>
+      </c>
+      <c r="FN45" s="16">
+        <v>7778978828</v>
+      </c>
+    </row>
+    <row r="46" spans="1:176" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -17513,8 +18825,26 @@
       <c r="ED46" s="16">
         <v>2601322552277</v>
       </c>
-    </row>
-    <row r="47" spans="1:156" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FI46" t="s">
+        <v>200</v>
+      </c>
+      <c r="FJ46" s="16">
+        <v>133079155737</v>
+      </c>
+      <c r="FK46" s="17">
+        <v>55662041</v>
+      </c>
+      <c r="FL46" s="17">
+        <v>24795219</v>
+      </c>
+      <c r="FM46" s="16">
+        <v>99528869971</v>
+      </c>
+      <c r="FN46" s="16">
+        <v>65633478739</v>
+      </c>
+    </row>
+    <row r="47" spans="1:176" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -17584,8 +18914,26 @@
       <c r="ED47" s="16">
         <v>2488808669602</v>
       </c>
-    </row>
-    <row r="48" spans="1:156" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="FI47" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="FJ47" s="16">
+        <v>2392936011460</v>
+      </c>
+      <c r="FK47" s="17">
+        <v>499437562</v>
+      </c>
+      <c r="FL47" s="17">
+        <v>241397897</v>
+      </c>
+      <c r="FM47" s="16">
+        <v>2147746588007</v>
+      </c>
+      <c r="FN47" s="16">
+        <v>1267188978449</v>
+      </c>
+    </row>
+    <row r="48" spans="1:176" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -28982,16 +30330,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A83:I83"/>
+    <mergeCell ref="A91:I91"/>
+    <mergeCell ref="A99:I99"/>
+    <mergeCell ref="A42:I42"/>
     <mergeCell ref="K4:S4"/>
     <mergeCell ref="K19:S19"/>
     <mergeCell ref="A106:I106"/>
     <mergeCell ref="A122:I122"/>
     <mergeCell ref="A105:I105"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A83:I83"/>
-    <mergeCell ref="A91:I91"/>
-    <mergeCell ref="A99:I99"/>
-    <mergeCell ref="A42:I42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>